<commit_message>
Jar prepared for post-processing
</commit_message>
<xml_diff>
--- a/ProteinPipelineScripts/resources/UMOD_TABLE.xlsx
+++ b/ProteinPipelineScripts/resources/UMOD_TABLE.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="20" windowWidth="18980" windowHeight="11960"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15560"/>
   </bookViews>
   <sheets>
     <sheet name="UMOD_TABLE" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="149">
   <si>
     <t>umod name</t>
   </si>
@@ -179,9 +179,6 @@
     <t>avg mass</t>
   </si>
   <si>
-    <t>Acetyl(Protein N-term)</t>
-  </si>
-  <si>
     <t>Protein N-term</t>
   </si>
   <si>
@@ -191,9 +188,6 @@
     <t>N-term</t>
   </si>
   <si>
-    <t>Acetyl(K)</t>
-  </si>
-  <si>
     <t>K</t>
   </si>
   <si>
@@ -203,15 +197,9 @@
     <t>Protein C-term</t>
   </si>
   <si>
-    <t>Amidated(C-term)</t>
-  </si>
-  <si>
     <t>C-term</t>
   </si>
   <si>
-    <t>Ammonia-loss(N-term C)</t>
-  </si>
-  <si>
     <t>N-term C</t>
   </si>
   <si>
@@ -221,21 +209,9 @@
     <t>Biotin(K)</t>
   </si>
   <si>
-    <t>Carbamidomethyl(C)</t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
-    <t>Carbamyl(N-term)</t>
-  </si>
-  <si>
-    <t>Carbamyl(K)</t>
-  </si>
-  <si>
-    <t>Carboxymethyl(C)</t>
-  </si>
-  <si>
     <t>Cation:Na(D)</t>
   </si>
   <si>
@@ -251,15 +227,9 @@
     <t>E</t>
   </si>
   <si>
-    <t>Deamidated(N)</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
-    <t>Deamidated(Q)</t>
-  </si>
-  <si>
     <t>Q</t>
   </si>
   <si>
@@ -269,9 +239,6 @@
     <t>Dehydro(C)</t>
   </si>
   <si>
-    <t>Dioxidation(M)</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
@@ -284,15 +251,6 @@
     <t>ExacTagThiol(C)</t>
   </si>
   <si>
-    <t>Formyl(Protein N-term)</t>
-  </si>
-  <si>
-    <t>Formyl(N-term)</t>
-  </si>
-  <si>
-    <t>Glu-&gt;pyro-Glu(N-term E)</t>
-  </si>
-  <si>
     <t>N-term E</t>
   </si>
   <si>
@@ -302,15 +260,6 @@
     <t>N-term Q</t>
   </si>
   <si>
-    <t>Guanidinyl(K)</t>
-  </si>
-  <si>
-    <t>ICAT-C(C)</t>
-  </si>
-  <si>
-    <t>ICAT-C:13C(9)(C)</t>
-  </si>
-  <si>
     <t>ICPL(Protein N-term)</t>
   </si>
   <si>
@@ -338,54 +287,12 @@
     <t>ICPL:2H(4)(K)</t>
   </si>
   <si>
-    <t>iTRAQ4plex(N-term)</t>
-  </si>
-  <si>
-    <t>iTRAQ4plex(K)</t>
-  </si>
-  <si>
-    <t>iTRAQ4plex(Y)</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
-    <t>iTRAQ8plex(Y)</t>
-  </si>
-  <si>
-    <t>iTRAQ8plex(N-term)</t>
-  </si>
-  <si>
-    <t>iTRAQ8plex(K)</t>
-  </si>
-  <si>
-    <t>Label:18O(1)(C-term)</t>
-  </si>
-  <si>
-    <t>Label:18O(2)(C-term)</t>
-  </si>
-  <si>
-    <t>Met-&gt;Hse(C-term M)</t>
-  </si>
-  <si>
     <t>C-term M</t>
   </si>
   <si>
-    <t>Met-&gt;Hsl(C-term M)</t>
-  </si>
-  <si>
-    <t>Methyl(C-term)</t>
-  </si>
-  <si>
-    <t>Methyl(D)</t>
-  </si>
-  <si>
-    <t>Methyl(E)</t>
-  </si>
-  <si>
-    <t>Methylthio(C)</t>
-  </si>
-  <si>
     <t>mTRAQ(Y)</t>
   </si>
   <si>
@@ -404,51 +311,21 @@
     <t>mTRAQ:13C(3)15N(1)(Y)</t>
   </si>
   <si>
-    <t>NIPCAM(C)</t>
-  </si>
-  <si>
-    <t>Oxidation(W)</t>
-  </si>
-  <si>
     <t>W</t>
   </si>
   <si>
-    <t>Oxidation(H)</t>
-  </si>
-  <si>
     <t>H</t>
   </si>
   <si>
-    <t>Oxidation(M)</t>
-  </si>
-  <si>
-    <t>Phospho(Y)</t>
-  </si>
-  <si>
-    <t>Phospho(T)</t>
-  </si>
-  <si>
     <t>T</t>
   </si>
   <si>
-    <t>Phospho(S)</t>
-  </si>
-  <si>
     <t>S</t>
   </si>
   <si>
-    <t>Propionamide(C)</t>
-  </si>
-  <si>
-    <t>Pyridylethyl(C)</t>
-  </si>
-  <si>
     <t>Pyro-carbamidomethyl(N-term C)</t>
   </si>
   <si>
-    <t>Sulfo(Y)</t>
-  </si>
-  <si>
     <t>Sulfo(T)</t>
   </si>
   <si>
@@ -461,23 +338,143 @@
     <t>TMT(K)</t>
   </si>
   <si>
-    <t>TMT2plex(N-term)</t>
-  </si>
-  <si>
-    <t>TMT2plex(K)</t>
-  </si>
-  <si>
-    <t>TMT6plex(N-term)</t>
-  </si>
-  <si>
-    <t>TMT6plex(K)</t>
+    <t>acetylation of protein n-term</t>
+  </si>
+  <si>
+    <t>acetylation of K</t>
+  </si>
+  <si>
+    <t>amidation of peptide c-term</t>
+  </si>
+  <si>
+    <t>pyro-glu from n-term Q</t>
+  </si>
+  <si>
+    <t>carbamidomethyl C</t>
+  </si>
+  <si>
+    <t>carbamylation of n-term peptide</t>
+  </si>
+  <si>
+    <t>carbamylation of K</t>
+  </si>
+  <si>
+    <t>carboxymethyl C</t>
+  </si>
+  <si>
+    <t>deamidation of N</t>
+  </si>
+  <si>
+    <t>deamidation of N and Q</t>
+  </si>
+  <si>
+    <t>sulphone of M</t>
+  </si>
+  <si>
+    <t>formylation of protein n-term</t>
+  </si>
+  <si>
+    <t>formylation of peptide n-term</t>
+  </si>
+  <si>
+    <t>pyro-glu from n-term E</t>
+  </si>
+  <si>
+    <t>guanidination of K</t>
+  </si>
+  <si>
+    <t>ICAT light</t>
+  </si>
+  <si>
+    <t>ICAT heavy</t>
+  </si>
+  <si>
+    <t>iTRAQ117 on nterm</t>
+  </si>
+  <si>
+    <t>iTRAQ117 on K</t>
+  </si>
+  <si>
+    <t>iTRAQ117 on Y</t>
+  </si>
+  <si>
+    <t>iTRAQ8plex:13C(7)15N(1) on Y</t>
+  </si>
+  <si>
+    <t>iTRAQ8plex:13C(7)15N(1) on nterm</t>
+  </si>
+  <si>
+    <t>iTRAQ8plex:13C(7)15N(1) on K</t>
+  </si>
+  <si>
+    <t>O18 on peptide n-term</t>
+  </si>
+  <si>
+    <t>di-O18 on peptide n-term</t>
+  </si>
+  <si>
+    <t>homoserine</t>
+  </si>
+  <si>
+    <t>homoserine lactone</t>
+  </si>
+  <si>
+    <t>methylation of peptide c-term</t>
+  </si>
+  <si>
+    <t>methylation of D</t>
+  </si>
+  <si>
+    <t>methylation of E</t>
+  </si>
+  <si>
+    <t>MMTS on C</t>
+  </si>
+  <si>
+    <t>oxidation of W</t>
+  </si>
+  <si>
+    <t>oxidation of H</t>
+  </si>
+  <si>
+    <t>oxidation of M</t>
+  </si>
+  <si>
+    <t>phosphorylation of Y</t>
+  </si>
+  <si>
+    <t>phosphorylation of T</t>
+  </si>
+  <si>
+    <t>phosphorylation of S</t>
+  </si>
+  <si>
+    <t>propionamide C</t>
+  </si>
+  <si>
+    <t>s-pyridylethylation of C</t>
+  </si>
+  <si>
+    <t>sulfation of Y</t>
+  </si>
+  <si>
+    <t>TMT duplex on n-term peptide</t>
+  </si>
+  <si>
+    <t>TMT 6-plex on K</t>
+  </si>
+  <si>
+    <t>TMT 6-plex on n-term peptide</t>
+  </si>
+  <si>
+    <t>TMT duplex on K</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="19">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -616,6 +613,22 @@
     <font>
       <sz val="8"/>
       <name val="Verdana"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -915,7 +928,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="140">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -958,56 +971,252 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="140">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent1 - 20%" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="Accent1 - 40%" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="Accent1 - 60%" xfId="21" builtinId="32" customBuiltin="1"/>
     <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent2 - 20%" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="Accent2 - 40%" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="Accent2 - 60%" xfId="25" builtinId="36" customBuiltin="1"/>
     <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent3 - 20%" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="Accent3 - 40%" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="Accent3 - 60%" xfId="29" builtinId="40" customBuiltin="1"/>
     <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent4 - 20%" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="Accent4 - 40%" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="Accent4 - 60%" xfId="33" builtinId="44" customBuiltin="1"/>
     <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent5 - 20%" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="Accent5 - 40%" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="Accent5 - 60%" xfId="37" builtinId="48" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Accent6 - 20%" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="Accent6 - 40%" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="Accent6 - 60%" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="134" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="136" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="138" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Sheet Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -1295,15 +1504,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="G79" sqref="G79"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="2" width="23.33203125" customWidth="1"/>
     <col min="3" max="3" width="20.33203125" customWidth="1"/>
@@ -1337,7 +1545,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
         <v>45</v>
@@ -1346,7 +1554,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E2">
         <v>42.010565</v>
@@ -1360,7 +1568,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -1369,7 +1577,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E3">
         <v>42.010565</v>
@@ -1380,7 +1588,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>106</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -1389,7 +1597,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E4">
         <v>42.010565</v>
@@ -1403,7 +1611,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -1412,7 +1620,7 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E5">
         <v>-0.984016</v>
@@ -1423,7 +1631,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>107</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
@@ -1432,7 +1640,7 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E6">
         <v>-0.984016</v>
@@ -1446,7 +1654,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>108</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
@@ -1455,7 +1663,7 @@
         <v>385</v>
       </c>
       <c r="D7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E7">
         <v>-17.026548999999999</v>
@@ -1469,7 +1677,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
@@ -1478,7 +1686,7 @@
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E8">
         <v>226.07759799999999</v>
@@ -1489,7 +1697,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B9" t="s">
         <v>4</v>
@@ -1498,7 +1706,7 @@
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E9">
         <v>226.07759799999999</v>
@@ -1509,7 +1717,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>109</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
@@ -1518,7 +1726,7 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E10">
         <v>57.021464000000002</v>
@@ -1532,7 +1740,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>110</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
@@ -1541,7 +1749,7 @@
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E11">
         <v>43.005814000000001</v>
@@ -1555,7 +1763,7 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>69</v>
+        <v>111</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
@@ -1564,7 +1772,7 @@
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E12">
         <v>43.005814000000001</v>
@@ -1578,7 +1786,7 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>112</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
@@ -1587,7 +1795,7 @@
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E13">
         <v>58.005479000000001</v>
@@ -1601,7 +1809,7 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
@@ -1610,7 +1818,7 @@
         <v>30</v>
       </c>
       <c r="D14" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E14">
         <v>21.981943000000001</v>
@@ -1621,7 +1829,7 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
@@ -1630,7 +1838,7 @@
         <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E15">
         <v>21.981943000000001</v>
@@ -1641,7 +1849,7 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B16" t="s">
         <v>8</v>
@@ -1650,7 +1858,7 @@
         <v>30</v>
       </c>
       <c r="D16" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="E16">
         <v>21.981943000000001</v>
@@ -1661,7 +1869,7 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>76</v>
+        <v>113</v>
       </c>
       <c r="B17" t="s">
         <v>9</v>
@@ -1670,7 +1878,7 @@
         <v>7</v>
       </c>
       <c r="D17" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E17">
         <v>0.984016</v>
@@ -1684,7 +1892,7 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>78</v>
+        <v>114</v>
       </c>
       <c r="B18" t="s">
         <v>9</v>
@@ -1693,7 +1901,7 @@
         <v>7</v>
       </c>
       <c r="D18" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="E18">
         <v>0.984016</v>
@@ -1707,7 +1915,7 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
@@ -1716,7 +1924,7 @@
         <v>23</v>
       </c>
       <c r="D19" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E19">
         <v>-18.010565</v>
@@ -1727,7 +1935,7 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="B20" t="s">
         <v>11</v>
@@ -1736,7 +1944,7 @@
         <v>374</v>
       </c>
       <c r="D20" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E20">
         <v>-1.007825</v>
@@ -1747,7 +1955,7 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>82</v>
+        <v>115</v>
       </c>
       <c r="B21" t="s">
         <v>12</v>
@@ -1756,7 +1964,7 @@
         <v>425</v>
       </c>
       <c r="D21" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="E21">
         <v>31.989829</v>
@@ -1770,7 +1978,7 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B22" t="s">
         <v>13</v>
@@ -1779,7 +1987,7 @@
         <v>278</v>
       </c>
       <c r="D22" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E22">
         <v>44.026215000000001</v>
@@ -1790,7 +1998,7 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="B23" t="s">
         <v>14</v>
@@ -1799,7 +2007,7 @@
         <v>741</v>
       </c>
       <c r="D23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E23">
         <v>1030.35294</v>
@@ -1810,7 +2018,7 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B24" t="s">
         <v>15</v>
@@ -1819,7 +2027,7 @@
         <v>740</v>
       </c>
       <c r="D24" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E24">
         <v>972.36521900000002</v>
@@ -1830,7 +2038,7 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>87</v>
+        <v>116</v>
       </c>
       <c r="B25" t="s">
         <v>16</v>
@@ -1839,7 +2047,7 @@
         <v>122</v>
       </c>
       <c r="D25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E25">
         <v>27.994914999999999</v>
@@ -1853,7 +2061,7 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>88</v>
+        <v>117</v>
       </c>
       <c r="B26" t="s">
         <v>16</v>
@@ -1862,7 +2070,7 @@
         <v>122</v>
       </c>
       <c r="D26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E26">
         <v>27.994914999999999</v>
@@ -1876,7 +2084,7 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>89</v>
+        <v>118</v>
       </c>
       <c r="B27" t="s">
         <v>17</v>
@@ -1885,7 +2093,7 @@
         <v>27</v>
       </c>
       <c r="D27" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="E27">
         <v>-18.010565</v>
@@ -1899,7 +2107,7 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="B28" t="s">
         <v>17</v>
@@ -1908,7 +2116,7 @@
         <v>28</v>
       </c>
       <c r="D28" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="E28">
         <v>-17.026548999999999</v>
@@ -1919,7 +2127,7 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="B29" t="s">
         <v>18</v>
@@ -1928,7 +2136,7 @@
         <v>52</v>
       </c>
       <c r="D29" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E29">
         <v>42.021797999999997</v>
@@ -1942,7 +2150,7 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>94</v>
+        <v>120</v>
       </c>
       <c r="B30" t="s">
         <v>19</v>
@@ -1951,7 +2159,7 @@
         <v>105</v>
       </c>
       <c r="D30" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E30">
         <v>227.126991</v>
@@ -1965,7 +2173,7 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>95</v>
+        <v>121</v>
       </c>
       <c r="B31" t="s">
         <v>20</v>
@@ -1974,7 +2182,7 @@
         <v>106</v>
       </c>
       <c r="D31" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E31">
         <v>236.157185</v>
@@ -1988,7 +2196,7 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="B32" t="s">
         <v>21</v>
@@ -1997,7 +2205,7 @@
         <v>365</v>
       </c>
       <c r="D32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E32">
         <v>105.02146399999999</v>
@@ -2008,7 +2216,7 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="B33" t="s">
         <v>21</v>
@@ -2017,7 +2225,7 @@
         <v>365</v>
       </c>
       <c r="D33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E33">
         <v>105.02146399999999</v>
@@ -2028,7 +2236,7 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="B34" t="s">
         <v>22</v>
@@ -2037,7 +2245,7 @@
         <v>364</v>
       </c>
       <c r="D34" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E34">
         <v>111.04159300000001</v>
@@ -2048,7 +2256,7 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="B35" t="s">
         <v>22</v>
@@ -2057,7 +2265,7 @@
         <v>364</v>
       </c>
       <c r="D35" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E35">
         <v>111.04159300000001</v>
@@ -2068,7 +2276,7 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="B36" t="s">
         <v>23</v>
@@ -2077,7 +2285,7 @@
         <v>866</v>
       </c>
       <c r="D36" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E36">
         <v>115.0667</v>
@@ -2088,7 +2296,7 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="B37" t="s">
         <v>23</v>
@@ -2097,7 +2305,7 @@
         <v>866</v>
       </c>
       <c r="D37" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E37">
         <v>115.0667</v>
@@ -2108,7 +2316,7 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="B38" t="s">
         <v>23</v>
@@ -2117,7 +2325,7 @@
         <v>866</v>
       </c>
       <c r="D38" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E38">
         <v>115.0667</v>
@@ -2128,7 +2336,7 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="B39" t="s">
         <v>24</v>
@@ -2137,7 +2345,7 @@
         <v>687</v>
       </c>
       <c r="D39" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E39">
         <v>109.046571</v>
@@ -2148,7 +2356,7 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="B40" t="s">
         <v>24</v>
@@ -2157,7 +2365,7 @@
         <v>687</v>
       </c>
       <c r="D40" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E40">
         <v>109.046571</v>
@@ -2168,7 +2376,7 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
-        <v>105</v>
+        <v>122</v>
       </c>
       <c r="B41" t="s">
         <v>25</v>
@@ -2177,7 +2385,7 @@
         <v>214</v>
       </c>
       <c r="D41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E41">
         <v>144.10206299999999</v>
@@ -2191,7 +2399,7 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="B42" t="s">
         <v>25</v>
@@ -2200,7 +2408,7 @@
         <v>214</v>
       </c>
       <c r="D42" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E42">
         <v>144.10206299999999</v>
@@ -2214,7 +2422,7 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" t="s">
-        <v>107</v>
+        <v>124</v>
       </c>
       <c r="B43" t="s">
         <v>25</v>
@@ -2223,7 +2431,7 @@
         <v>214</v>
       </c>
       <c r="D43" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="E43">
         <v>144.10206299999999</v>
@@ -2237,7 +2445,7 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="B44" t="s">
         <v>26</v>
@@ -2246,7 +2454,7 @@
         <v>730</v>
       </c>
       <c r="D44" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="E44">
         <v>304.20535999999998</v>
@@ -2260,7 +2468,7 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="B45" t="s">
         <v>26</v>
@@ -2269,7 +2477,7 @@
         <v>730</v>
       </c>
       <c r="D45" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E45">
         <v>304.20535999999998</v>
@@ -2283,7 +2491,7 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="B46" t="s">
         <v>26</v>
@@ -2292,7 +2500,7 @@
         <v>730</v>
       </c>
       <c r="D46" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E46">
         <v>304.20535999999998</v>
@@ -2306,7 +2514,7 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="B47" t="s">
         <v>27</v>
@@ -2315,7 +2523,7 @@
         <v>258</v>
       </c>
       <c r="D47" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E47">
         <v>2.0042460000000002</v>
@@ -2329,7 +2537,7 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="B48" t="s">
         <v>28</v>
@@ -2338,7 +2546,7 @@
         <v>193</v>
       </c>
       <c r="D48" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E48">
         <v>4.0084910000000002</v>
@@ -2352,7 +2560,7 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
       <c r="B49" t="s">
         <v>29</v>
@@ -2361,7 +2569,7 @@
         <v>10</v>
       </c>
       <c r="D49" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="E49">
         <v>-29.992806000000002</v>
@@ -2375,7 +2583,7 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>116</v>
+        <v>131</v>
       </c>
       <c r="B50" t="s">
         <v>30</v>
@@ -2384,7 +2592,7 @@
         <v>11</v>
       </c>
       <c r="D50" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="E50">
         <v>-48.003371000000001</v>
@@ -2398,7 +2606,7 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" t="s">
-        <v>117</v>
+        <v>132</v>
       </c>
       <c r="B51" t="s">
         <v>31</v>
@@ -2407,7 +2615,7 @@
         <v>34</v>
       </c>
       <c r="D51" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E51">
         <v>14.015650000000001</v>
@@ -2421,7 +2629,7 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" t="s">
-        <v>118</v>
+        <v>133</v>
       </c>
       <c r="B52" t="s">
         <v>31</v>
@@ -2430,7 +2638,7 @@
         <v>34</v>
       </c>
       <c r="D52" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E52">
         <v>14.015650000000001</v>
@@ -2444,7 +2652,7 @@
     </row>
     <row r="53" spans="1:7">
       <c r="A53" t="s">
-        <v>119</v>
+        <v>134</v>
       </c>
       <c r="B53" t="s">
         <v>31</v>
@@ -2453,7 +2661,7 @@
         <v>34</v>
       </c>
       <c r="D53" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="E53">
         <v>14.015650000000001</v>
@@ -2467,7 +2675,7 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" t="s">
-        <v>120</v>
+        <v>135</v>
       </c>
       <c r="B54" t="s">
         <v>32</v>
@@ -2476,7 +2684,7 @@
         <v>39</v>
       </c>
       <c r="D54" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E54">
         <v>45.987721000000001</v>
@@ -2490,7 +2698,7 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" t="s">
-        <v>121</v>
+        <v>90</v>
       </c>
       <c r="B55" t="s">
         <v>33</v>
@@ -2499,7 +2707,7 @@
         <v>888</v>
       </c>
       <c r="D55" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="E55">
         <v>140.09496300000001</v>
@@ -2510,7 +2718,7 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" t="s">
-        <v>122</v>
+        <v>91</v>
       </c>
       <c r="B56" t="s">
         <v>33</v>
@@ -2519,7 +2727,7 @@
         <v>888</v>
       </c>
       <c r="D56" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E56">
         <v>140.09496300000001</v>
@@ -2530,7 +2738,7 @@
     </row>
     <row r="57" spans="1:7">
       <c r="A57" t="s">
-        <v>123</v>
+        <v>92</v>
       </c>
       <c r="B57" t="s">
         <v>33</v>
@@ -2539,7 +2747,7 @@
         <v>888</v>
       </c>
       <c r="D57" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E57">
         <v>140.09496300000001</v>
@@ -2550,7 +2758,7 @@
     </row>
     <row r="58" spans="1:7">
       <c r="A58" t="s">
-        <v>124</v>
+        <v>93</v>
       </c>
       <c r="B58" t="s">
         <v>34</v>
@@ -2559,7 +2767,7 @@
         <v>889</v>
       </c>
       <c r="D58" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E58">
         <v>144.10206299999999</v>
@@ -2570,7 +2778,7 @@
     </row>
     <row r="59" spans="1:7">
       <c r="A59" t="s">
-        <v>125</v>
+        <v>94</v>
       </c>
       <c r="B59" t="s">
         <v>34</v>
@@ -2579,7 +2787,7 @@
         <v>889</v>
       </c>
       <c r="D59" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E59">
         <v>144.10206299999999</v>
@@ -2590,7 +2798,7 @@
     </row>
     <row r="60" spans="1:7">
       <c r="A60" t="s">
-        <v>126</v>
+        <v>95</v>
       </c>
       <c r="B60" t="s">
         <v>34</v>
@@ -2599,7 +2807,7 @@
         <v>889</v>
       </c>
       <c r="D60" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="E60">
         <v>144.10206299999999</v>
@@ -2610,7 +2818,7 @@
     </row>
     <row r="61" spans="1:7">
       <c r="A61" t="s">
-        <v>127</v>
+        <v>35</v>
       </c>
       <c r="B61" t="s">
         <v>35</v>
@@ -2619,7 +2827,7 @@
         <v>17</v>
       </c>
       <c r="D61" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E61">
         <v>99.068414000000004</v>
@@ -2633,7 +2841,7 @@
     </row>
     <row r="62" spans="1:7">
       <c r="A62" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="B62" t="s">
         <v>36</v>
@@ -2642,7 +2850,7 @@
         <v>35</v>
       </c>
       <c r="D62" t="s">
-        <v>129</v>
+        <v>96</v>
       </c>
       <c r="E62">
         <v>15.994915000000001</v>
@@ -2656,7 +2864,7 @@
     </row>
     <row r="63" spans="1:7">
       <c r="A63" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="B63" t="s">
         <v>36</v>
@@ -2665,7 +2873,7 @@
         <v>35</v>
       </c>
       <c r="D63" t="s">
-        <v>131</v>
+        <v>97</v>
       </c>
       <c r="E63">
         <v>15.994915000000001</v>
@@ -2679,7 +2887,7 @@
     </row>
     <row r="64" spans="1:7">
       <c r="A64" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="B64" t="s">
         <v>36</v>
@@ -2688,7 +2896,7 @@
         <v>35</v>
       </c>
       <c r="D64" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="E64">
         <v>15.994915000000001</v>
@@ -2702,7 +2910,7 @@
     </row>
     <row r="65" spans="1:7">
       <c r="A65" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="B65" t="s">
         <v>37</v>
@@ -2711,7 +2919,7 @@
         <v>21</v>
       </c>
       <c r="D65" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="E65">
         <v>79.966330999999997</v>
@@ -2725,7 +2933,7 @@
     </row>
     <row r="66" spans="1:7">
       <c r="A66" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="B66" t="s">
         <v>37</v>
@@ -2734,7 +2942,7 @@
         <v>21</v>
       </c>
       <c r="D66" t="s">
-        <v>135</v>
+        <v>98</v>
       </c>
       <c r="E66">
         <v>79.966330999999997</v>
@@ -2748,7 +2956,7 @@
     </row>
     <row r="67" spans="1:7">
       <c r="A67" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="B67" t="s">
         <v>37</v>
@@ -2757,7 +2965,7 @@
         <v>21</v>
       </c>
       <c r="D67" t="s">
-        <v>137</v>
+        <v>99</v>
       </c>
       <c r="E67">
         <v>79.966330999999997</v>
@@ -2771,7 +2979,7 @@
     </row>
     <row r="68" spans="1:7">
       <c r="A68" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B68" t="s">
         <v>38</v>
@@ -2780,7 +2988,7 @@
         <v>24</v>
       </c>
       <c r="D68" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E68">
         <v>71.037114000000003</v>
@@ -2794,7 +3002,7 @@
     </row>
     <row r="69" spans="1:7">
       <c r="A69" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="B69" t="s">
         <v>39</v>
@@ -2803,7 +3011,7 @@
         <v>31</v>
       </c>
       <c r="D69" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E69">
         <v>105.057849</v>
@@ -2817,7 +3025,7 @@
     </row>
     <row r="70" spans="1:7">
       <c r="A70" t="s">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="B70" t="s">
         <v>40</v>
@@ -2826,7 +3034,7 @@
         <v>26</v>
       </c>
       <c r="D70" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E70">
         <v>39.994914999999999</v>
@@ -2837,7 +3045,7 @@
     </row>
     <row r="71" spans="1:7">
       <c r="A71" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B71" t="s">
         <v>41</v>
@@ -2846,7 +3054,7 @@
         <v>40</v>
       </c>
       <c r="D71" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="E71">
         <v>79.956815000000006</v>
@@ -2860,7 +3068,7 @@
     </row>
     <row r="72" spans="1:7">
       <c r="A72" t="s">
-        <v>142</v>
+        <v>101</v>
       </c>
       <c r="B72" t="s">
         <v>41</v>
@@ -2869,7 +3077,7 @@
         <v>40</v>
       </c>
       <c r="D72" t="s">
-        <v>135</v>
+        <v>98</v>
       </c>
       <c r="E72">
         <v>79.956815000000006</v>
@@ -2880,7 +3088,7 @@
     </row>
     <row r="73" spans="1:7">
       <c r="A73" t="s">
-        <v>143</v>
+        <v>102</v>
       </c>
       <c r="B73" t="s">
         <v>41</v>
@@ -2889,7 +3097,7 @@
         <v>40</v>
       </c>
       <c r="D73" t="s">
-        <v>137</v>
+        <v>99</v>
       </c>
       <c r="E73">
         <v>79.956815000000006</v>
@@ -2900,7 +3108,7 @@
     </row>
     <row r="74" spans="1:7">
       <c r="A74" t="s">
-        <v>144</v>
+        <v>103</v>
       </c>
       <c r="B74" t="s">
         <v>42</v>
@@ -2909,7 +3117,7 @@
         <v>739</v>
       </c>
       <c r="D74" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E74">
         <v>224.152478</v>
@@ -2920,7 +3128,7 @@
     </row>
     <row r="75" spans="1:7">
       <c r="A75" t="s">
-        <v>145</v>
+        <v>104</v>
       </c>
       <c r="B75" t="s">
         <v>42</v>
@@ -2929,7 +3137,7 @@
         <v>739</v>
       </c>
       <c r="D75" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E75">
         <v>224.152478</v>
@@ -2940,7 +3148,7 @@
     </row>
     <row r="76" spans="1:7">
       <c r="A76" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B76" t="s">
         <v>43</v>
@@ -2949,7 +3157,7 @@
         <v>738</v>
       </c>
       <c r="D76" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E76">
         <v>225.155833</v>
@@ -2963,7 +3171,7 @@
     </row>
     <row r="77" spans="1:7">
       <c r="A77" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B77" t="s">
         <v>43</v>
@@ -2972,7 +3180,7 @@
         <v>738</v>
       </c>
       <c r="D77" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E77">
         <v>225.155833</v>
@@ -2986,7 +3194,7 @@
     </row>
     <row r="78" spans="1:7">
       <c r="A78" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B78" t="s">
         <v>44</v>
@@ -2995,7 +3203,7 @@
         <v>737</v>
       </c>
       <c r="D78" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E78">
         <v>229.16293200000001</v>
@@ -3009,7 +3217,7 @@
     </row>
     <row r="79" spans="1:7">
       <c r="A79" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B79" t="s">
         <v>44</v>
@@ -3018,7 +3226,7 @@
         <v>737</v>
       </c>
       <c r="D79" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E79">
         <v>229.16293200000001</v>
@@ -3031,12 +3239,11 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>